<commit_message>
whalla plein de truc
</commit_message>
<xml_diff>
--- a/resultats.xlsx
+++ b/resultats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stani\Documents\modal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F415E076-6E92-4A04-B5F4-5BDE9A98AF00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79E67E3-8B30-44ED-A78A-7C053C70174A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22332" yWindow="576" windowWidth="21600" windowHeight="11328" xr2:uid="{8DC7B937-7C08-4534-888D-7BA5F8F9BAED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DC7B937-7C08-4534-888D-7BA5F8F9BAED}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Modèle / dataset</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>100_120</t>
-  </si>
-  <si>
-    <t>200_120</t>
   </si>
   <si>
     <t>sup150</t>
@@ -446,17 +443,17 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,18 +463,16 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -496,7 +491,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -515,7 +510,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -536,9 +531,9 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>0.93</v>
@@ -557,9 +552,9 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>0.85</v>
@@ -568,7 +563,7 @@
         <v>0.78</v>
       </c>
       <c r="D6" s="1">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
@@ -576,9 +571,9 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>0.86</v>
@@ -594,7 +589,7 @@
         <v>0.72</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>